<commit_message>
Fix BOM in release R01
</commit_message>
<xml_diff>
--- a/releases/candlelight-S01-R01/candlelight-S01-R01-V01/BOM/candleLight-S01-R01-V01.xlsx
+++ b/releases/candlelight-S01-R01/candlelight-S01-R01-V01/BOM/candleLight-S01-R01-V01.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="83">
   <si>
     <t xml:space="preserve">Company: Linux Automation GmbH</t>
   </si>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Release-State: released</t>
   </si>
   <si>
-    <t xml:space="preserve">Release-Date: 2021-03-03</t>
+    <t xml:space="preserve">Release-Date: 2021-04-07</t>
   </si>
   <si>
     <t xml:space="preserve">count</t>
@@ -76,19 +76,13 @@
     <t xml:space="preserve">libsource</t>
   </si>
   <si>
-    <t xml:space="preserve">tstamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C403, C206, C301, C204, C205, C208, C207, C402, C303, C203</t>
+    <t xml:space="preserve">C301, C207, C303</t>
   </si>
   <si>
     <t xml:space="preserve">nan</t>
   </si>
   <si>
-    <t xml:space="preserve">C_Small, 10uF, 100nF</t>
+    <t xml:space="preserve">10uF</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -100,7 +94,7 @@
     <t xml:space="preserve">all</t>
   </si>
   <si>
-    <t xml:space="preserve">nan, Capacitors_SMD:C_0603, Capacitors_SMD:C_0805</t>
+    <t xml:space="preserve">Capacitors_SMD:C_0805</t>
   </si>
   <si>
     <t xml:space="preserve">C</t>
@@ -109,25 +103,28 @@
     <t xml:space="preserve">candleLight-rescue:C_Small</t>
   </si>
   <si>
-    <t xml:space="preserve">56F5A44C, 56F5410C, 56F540FA, 56F611D6, 56F5404F, 56F54256, 57225548, 56F53D48, 56F60BBB, 56F5A3FD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D603, D601, D602</t>
+    <t xml:space="preserve">C203, C204, C205, C206,C208, C402, C403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100nF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacitors_SMD:C_0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D601</t>
   </si>
   <si>
     <t xml:space="preserve">Kingbright</t>
   </si>
   <si>
-    <t xml:space="preserve">APT1608EC, APT1608YC, APT1608SGC</t>
+    <t xml:space="preserve">APT1608SGC</t>
   </si>
   <si>
     <t xml:space="preserve">LED</t>
   </si>
   <si>
-    <t xml:space="preserve">nan, LEDs:LED_0603</t>
+    <t xml:space="preserve">LEDs:LED_0603</t>
   </si>
   <si>
     <t xml:space="preserve">D</t>
@@ -136,10 +133,37 @@
     <t xml:space="preserve">candleLight-rescue:LED</t>
   </si>
   <si>
-    <t xml:space="preserve">56F5F923, 56F5F775, 56F5F971</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.0</t>
+    <t xml:space="preserve">D602</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APT1608YC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APT1608EC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM32F072C8T6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STM32F072C8Tx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LQFP48, Housings_QFP:LQFP-48_7x7mm_Pitch0.5mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">candleLight-rescue:STM32F072C8Tx</t>
   </si>
   <si>
     <t xml:space="preserve">U301</t>
@@ -154,28 +178,19 @@
     <t xml:space="preserve">MCP1754ST-3302E/MB, MCP1754ST-3302E_MB</t>
   </si>
   <si>
-    <t xml:space="preserve">nan, TO_SOT_Packages_SMD:SOT89-3_Housing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U</t>
+    <t xml:space="preserve">TO_SOT_Packages_SMD:SOT89-3_Housing</t>
   </si>
   <si>
     <t xml:space="preserve">candleLight-rescue:MCP1754ST-3302E_MB</t>
   </si>
   <si>
-    <t xml:space="preserve">56F609E7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R602, R603, R201, R204, R601, R202, R401</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R, 1K, 4K7, 10K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nan, Resistors_SMD:R_0603</t>
+    <t xml:space="preserve">R201, R202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4K7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistors_SMD:R_0603</t>
   </si>
   <si>
     <t xml:space="preserve">R</t>
@@ -184,28 +199,16 @@
     <t xml:space="preserve">candleLight-rescue:R</t>
   </si>
   <si>
-    <t xml:space="preserve">56F50E38, 56F69C0C, 56F67521, 56F67576, 56F67763, 56F50945, 56F508B6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U201</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM32F072C8T6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM32F072C8Tx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LQFP48, Housings_QFP:LQFP-48_7x7mm_Pitch0.5mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">candleLight-rescue:STM32F072C8Tx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56F46EB5</t>
+    <t xml:space="preserve">R204, R601, R602, R603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R401</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10K</t>
   </si>
   <si>
     <t xml:space="preserve">X502</t>
@@ -220,7 +223,7 @@
     <t xml:space="preserve">SUB-D9</t>
   </si>
   <si>
-    <t xml:space="preserve">nan, Connect:DB9M_CI</t>
+    <t xml:space="preserve">Connect:DB9M_CI</t>
   </si>
   <si>
     <t xml:space="preserve">X</t>
@@ -229,9 +232,6 @@
     <t xml:space="preserve">candleLight-rescue:SUB-D9</t>
   </si>
   <si>
-    <t xml:space="preserve">56F5D127</t>
-  </si>
-  <si>
     <t xml:space="preserve">U401</t>
   </si>
   <si>
@@ -244,15 +244,12 @@
     <t xml:space="preserve">TJA1051_3, TJA1051/3</t>
   </si>
   <si>
-    <t xml:space="preserve">nan, Housings_SOIC:SOIC-8_3.9x4.9mm_Pitch1.27mm</t>
+    <t xml:space="preserve">Housings_SOIC:SOIC-8_3.9x4.9mm_Pitch1.27mm</t>
   </si>
   <si>
     <t xml:space="preserve">candleLight-rescue:TJA1051_3</t>
   </si>
   <si>
-    <t xml:space="preserve">56F5A273</t>
-  </si>
-  <si>
     <t xml:space="preserve">P501</t>
   </si>
   <si>
@@ -265,16 +262,13 @@
     <t xml:space="preserve">USB_OTG</t>
   </si>
   <si>
-    <t xml:space="preserve">nan, usb:Molex-Micro-USB-B-Middle-Mount</t>
+    <t xml:space="preserve">usb:Molex-Micro-USB-B-Middle-Mount</t>
   </si>
   <si>
     <t xml:space="preserve">P</t>
   </si>
   <si>
     <t xml:space="preserve">candleLight-rescue:USB_OTG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56F68043</t>
   </si>
 </sst>
 </file>
@@ -355,12 +349,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -370,7 +364,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -379,18 +373,17 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="53.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="34.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="41.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="3.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="47.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="47.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="36.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="93.68"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -462,312 +455,460 @@
       <c r="K9" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="L9" s="0" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="0" t="s">
+      <c r="C10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="0" t="s">
+      <c r="F10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="0" t="s">
+      <c r="H10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="J10" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="K10" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="0" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="0" t="s">
+      <c r="C11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="0" t="s">
+      <c r="F11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="0" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="J11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="C12" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="D12" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="E12" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="F12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="0" t="s">
+      <c r="J12" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="K12" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="0" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="0" t="s">
+      <c r="C13" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="E13" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="C14" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="E14" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="C15" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="D15" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" s="0" t="s">
+      <c r="E15" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="J12" s="0" t="s">
+      <c r="F15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="K12" s="0" t="s">
+      <c r="J15" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="L12" s="0" t="s">
+      <c r="K15" s="0" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="C16" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="D16" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="0" t="s">
+      <c r="E16" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="F16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I16" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="K13" s="0" t="s">
+      <c r="J16" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K16" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="L13" s="0" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="0" t="s">
+      <c r="C17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="F17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="J17" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="K17" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="0" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="J14" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" s="0" t="s">
+      <c r="C18" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="L14" s="0" t="s">
+      <c r="F18" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="0" t="s">
+      <c r="C19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="F19" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="C20" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="D20" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" s="0" t="s">
+      <c r="E20" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="F20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="K15" s="0" t="s">
+      <c r="J20" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="L15" s="0" t="s">
+      <c r="K20" s="0" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="0" t="s">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C21" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D21" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E21" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" s="0" t="s">
+      <c r="F21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="J16" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="K16" s="0" t="s">
+      <c r="J21" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="L16" s="0" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="0" t="s">
+      <c r="C22" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="D22" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="E22" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="F22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="F17" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" s="0" t="s">
+      <c r="J22" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="J17" s="0" t="s">
+      <c r="K22" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="K17" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="L17" s="0" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>